<commit_message>
corr signals first checkin
</commit_message>
<xml_diff>
--- a/Data/usersDict.xlsx
+++ b/Data/usersDict.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -2146,9 +2146,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U89" sqref="U89"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCellId="1" sqref="O1:O1048576 A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4344,7 +4344,7 @@
         <v>252.09800000000001</v>
       </c>
       <c r="Y33" s="1">
-        <f t="shared" ref="Y32:Y40" si="9">ROUND(X33-P33, 3)</f>
+        <f t="shared" ref="Y33:Y40" si="9">ROUND(X33-P33, 3)</f>
         <v>3.2650000000000001</v>
       </c>
       <c r="AC33" s="1" t="s">
@@ -6895,7 +6895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
userDict didn't change only binary file changed
</commit_message>
<xml_diff>
--- a/Data/usersDict.xlsx
+++ b/Data/usersDict.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -2146,9 +2146,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCellId="1" sqref="O1:O1048576 A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6895,7 +6895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>